<commit_message>
Cleaning Up the code
</commit_message>
<xml_diff>
--- a/Project RP07 Letter.xlsx
+++ b/Project RP07 Letter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45988D9-0B52-428E-80FB-5468075630E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7FBE54-455B-4A74-B63A-3F77F016C50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,7 +408,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,6 +491,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -513,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -550,6 +558,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -835,9 +846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,13 +935,13 @@
       <c r="U1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="13" t="s">
         <v>90</v>
       </c>
       <c r="Y1" s="13" t="s">

</xml_diff>